<commit_message>
Update tabla de mortalidad
</commit_message>
<xml_diff>
--- a/Tasa de mortalidad.xlsx
+++ b/Tasa de mortalidad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moises Almanzar\Desktop\Proyecto Samsung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEBC5B20-3AC9-4EDE-B4A4-BD16D0D60976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{224D975D-1F7A-4076-BA85-854DBF86CE98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{40AD7953-8F09-4713-9AB9-62C2B40834AF}"/>
   </bookViews>
@@ -581,7 +581,7 @@
   <dimension ref="A1:C63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B2" sqref="B2:B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -605,7 +605,7 @@
         <v>2021</v>
       </c>
       <c r="B2" s="1">
-        <v>74.245000000000005</v>
+        <v>74245</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -616,7 +616,7 @@
         <v>2020</v>
       </c>
       <c r="B3" s="1">
-        <v>71.058000000000007</v>
+        <v>71058</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>4</v>
@@ -627,7 +627,7 @@
         <v>2019</v>
       </c>
       <c r="B4" s="1">
-        <v>62.21</v>
+        <v>6221</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
@@ -638,7 +638,7 @@
         <v>2018</v>
       </c>
       <c r="B5" s="1">
-        <v>62.212000000000003</v>
+        <v>62212</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>6</v>
@@ -649,7 +649,7 @@
         <v>2017</v>
       </c>
       <c r="B6" s="1">
-        <v>61.338999999999999</v>
+        <v>61339</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>7</v>
@@ -660,7 +660,7 @@
         <v>2016</v>
       </c>
       <c r="B7" s="1">
-        <v>60.087000000000003</v>
+        <v>60087</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>8</v>
@@ -671,7 +671,7 @@
         <v>2015</v>
       </c>
       <c r="B8" s="1">
-        <v>58.712000000000003</v>
+        <v>58712</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>9</v>
@@ -682,7 +682,7 @@
         <v>2014</v>
       </c>
       <c r="B9" s="1">
-        <v>57.588000000000001</v>
+        <v>57588</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>10</v>
@@ -693,7 +693,7 @@
         <v>2013</v>
       </c>
       <c r="B10" s="1">
-        <v>56.781999999999996</v>
+        <v>56782</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>11</v>
@@ -704,7 +704,7 @@
         <v>2012</v>
       </c>
       <c r="B11" s="1">
-        <v>56.168999999999997</v>
+        <v>56169</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>11</v>
@@ -715,7 +715,7 @@
         <v>2011</v>
       </c>
       <c r="B12" s="1">
-        <v>55.947000000000003</v>
+        <v>55947</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>12</v>
@@ -726,7 +726,7 @@
         <v>2010</v>
       </c>
       <c r="B13" s="1">
-        <v>55.177</v>
+        <v>55177</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>13</v>
@@ -737,7 +737,7 @@
         <v>2009</v>
       </c>
       <c r="B14" s="1">
-        <v>54.695</v>
+        <v>54695</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>10</v>
@@ -748,7 +748,7 @@
         <v>2008</v>
       </c>
       <c r="B15" s="1">
-        <v>54.112000000000002</v>
+        <v>54112</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>10</v>
@@ -759,7 +759,7 @@
         <v>2007</v>
       </c>
       <c r="B16" s="1">
-        <v>53.75</v>
+        <v>5375</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>14</v>
@@ -770,7 +770,7 @@
         <v>2006</v>
       </c>
       <c r="B17" s="1">
-        <v>53.274000000000001</v>
+        <v>53274</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>15</v>
@@ -781,7 +781,7 @@
         <v>2005</v>
       </c>
       <c r="B18" s="1">
-        <v>53.207000000000001</v>
+        <v>53207</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>16</v>
@@ -792,7 +792,7 @@
         <v>2004</v>
       </c>
       <c r="B19" s="1">
-        <v>53.936</v>
+        <v>53936</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>17</v>
@@ -803,7 +803,7 @@
         <v>2003</v>
       </c>
       <c r="B20" s="1">
-        <v>53.265999999999998</v>
+        <v>53266</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>17</v>
@@ -814,7 +814,7 @@
         <v>2002</v>
       </c>
       <c r="B21" s="1">
-        <v>53.511000000000003</v>
+        <v>53511</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>18</v>
@@ -825,7 +825,7 @@
         <v>2001</v>
       </c>
       <c r="B22" s="1">
-        <v>52.789000000000001</v>
+        <v>52789</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>18</v>
@@ -836,7 +836,7 @@
         <v>2000</v>
       </c>
       <c r="B23" s="1">
-        <v>51.807000000000002</v>
+        <v>51807</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>19</v>
@@ -847,7 +847,7 @@
         <v>1999</v>
       </c>
       <c r="B24" s="1">
-        <v>50.417000000000002</v>
+        <v>50417</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>17</v>
@@ -858,7 +858,7 @@
         <v>1998</v>
       </c>
       <c r="B25" s="1">
-        <v>49.116</v>
+        <v>49116</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>7</v>
@@ -869,7 +869,7 @@
         <v>1997</v>
       </c>
       <c r="B26" s="1">
-        <v>47.158999999999999</v>
+        <v>47159</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>9</v>
@@ -880,7 +880,7 @@
         <v>1996</v>
       </c>
       <c r="B27" s="1">
-        <v>45.676000000000002</v>
+        <v>45676</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>20</v>
@@ -891,7 +891,7 @@
         <v>1995</v>
       </c>
       <c r="B28" s="1">
-        <v>44.256</v>
+        <v>44256</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>21</v>
@@ -902,7 +902,7 @@
         <v>1994</v>
       </c>
       <c r="B29" s="1">
-        <v>42.978999999999999</v>
+        <v>42979</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>22</v>
@@ -913,7 +913,7 @@
         <v>1993</v>
       </c>
       <c r="B30" s="1">
-        <v>42.768000000000001</v>
+        <v>42768</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>23</v>
@@ -924,7 +924,7 @@
         <v>1992</v>
       </c>
       <c r="B31" s="1">
-        <v>42.701000000000001</v>
+        <v>42701</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>24</v>
@@ -935,7 +935,7 @@
         <v>1991</v>
       </c>
       <c r="B32" s="1">
-        <v>42.872999999999998</v>
+        <v>42873</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>25</v>
@@ -946,7 +946,7 @@
         <v>1990</v>
       </c>
       <c r="B33" s="1">
-        <v>43.262999999999998</v>
+        <v>43263</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>26</v>
@@ -957,7 +957,7 @@
         <v>1989</v>
       </c>
       <c r="B34" s="1">
-        <v>43.674999999999997</v>
+        <v>43675</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>27</v>
@@ -968,7 +968,7 @@
         <v>1988</v>
       </c>
       <c r="B35" s="1">
-        <v>44.054000000000002</v>
+        <v>44054</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>28</v>
@@ -979,7 +979,7 @@
         <v>1987</v>
       </c>
       <c r="B36" s="1">
-        <v>44.536000000000001</v>
+        <v>44536</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>3</v>
@@ -990,7 +990,7 @@
         <v>1986</v>
       </c>
       <c r="B37" s="1">
-        <v>45.179000000000002</v>
+        <v>45179</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>29</v>
@@ -1001,7 +1001,7 @@
         <v>1985</v>
       </c>
       <c r="B38" s="1">
-        <v>45.912999999999997</v>
+        <v>45913</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>30</v>
@@ -1012,7 +1012,7 @@
         <v>1984</v>
       </c>
       <c r="B39" s="1">
-        <v>46.664000000000001</v>
+        <v>46664</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>31</v>
@@ -1023,7 +1023,7 @@
         <v>1983</v>
       </c>
       <c r="B40" s="1">
-        <v>47.284999999999997</v>
+        <v>47285</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>32</v>
@@ -1034,7 +1034,7 @@
         <v>1982</v>
       </c>
       <c r="B41" s="1">
-        <v>47.825000000000003</v>
+        <v>47825</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>33</v>
@@ -1045,7 +1045,7 @@
         <v>1981</v>
       </c>
       <c r="B42" s="1">
-        <v>48.497</v>
+        <v>48497</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>34</v>
@@ -1056,7 +1056,7 @@
         <v>1980</v>
       </c>
       <c r="B43" s="1">
-        <v>49.24</v>
+        <v>4924</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>35</v>
@@ -1067,7 +1067,7 @@
         <v>1979</v>
       </c>
       <c r="B44" s="1">
-        <v>51.572000000000003</v>
+        <v>51572</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>36</v>
@@ -1078,7 +1078,7 @@
         <v>1978</v>
       </c>
       <c r="B45" s="1">
-        <v>50.101999999999997</v>
+        <v>50102</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>37</v>
@@ -1089,7 +1089,7 @@
         <v>1977</v>
       </c>
       <c r="B46" s="1">
-        <v>50.195999999999998</v>
+        <v>50196</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>38</v>
@@ -1100,7 +1100,7 @@
         <v>1976</v>
       </c>
       <c r="B47" s="1">
-        <v>50.343000000000004</v>
+        <v>50343</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>39</v>
@@ -1111,7 +1111,7 @@
         <v>1975</v>
       </c>
       <c r="B48" s="1">
-        <v>50.543999999999997</v>
+        <v>50544</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>40</v>
@@ -1122,7 +1122,7 @@
         <v>1974</v>
       </c>
       <c r="B49" s="1">
-        <v>50.820999999999998</v>
+        <v>50821</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>41</v>
@@ -1133,7 +1133,7 @@
         <v>1973</v>
       </c>
       <c r="B50" s="1">
-        <v>51.024999999999999</v>
+        <v>51025</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>42</v>
@@ -1144,7 +1144,7 @@
         <v>1972</v>
       </c>
       <c r="B51" s="1">
-        <v>51.066000000000003</v>
+        <v>51066</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>43</v>
@@ -1155,7 +1155,7 @@
         <v>1971</v>
       </c>
       <c r="B52" s="1">
-        <v>51.081000000000003</v>
+        <v>51081</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>44</v>
@@ -1166,7 +1166,7 @@
         <v>1970</v>
       </c>
       <c r="B53" s="1">
-        <v>51.436999999999998</v>
+        <v>51437</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>45</v>
@@ -1177,7 +1177,7 @@
         <v>1969</v>
       </c>
       <c r="B54" s="1">
-        <v>52.17</v>
+        <v>5217</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>46</v>
@@ -1188,7 +1188,7 @@
         <v>1968</v>
       </c>
       <c r="B55" s="1">
-        <v>52.941000000000003</v>
+        <v>52941</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>47</v>
@@ -1199,7 +1199,7 @@
         <v>1967</v>
       </c>
       <c r="B56" s="1">
-        <v>53.686999999999998</v>
+        <v>53687</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>48</v>
@@ -1210,7 +1210,7 @@
         <v>1966</v>
       </c>
       <c r="B57" s="1">
-        <v>54.3</v>
+        <v>543</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>49</v>
@@ -1221,7 +1221,7 @@
         <v>1965</v>
       </c>
       <c r="B58" s="1">
-        <v>58.564999999999998</v>
+        <v>58565</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>50</v>
@@ -1232,7 +1232,7 @@
         <v>1964</v>
       </c>
       <c r="B59" s="1">
-        <v>54.997999999999998</v>
+        <v>54998</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>51</v>
@@ -1243,7 +1243,7 @@
         <v>1963</v>
       </c>
       <c r="B60" s="1">
-        <v>55.704000000000001</v>
+        <v>55704</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>52</v>
@@ -1254,7 +1254,7 @@
         <v>1962</v>
       </c>
       <c r="B61" s="1">
-        <v>55.515000000000001</v>
+        <v>55515</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>53</v>
@@ -1265,7 +1265,7 @@
         <v>1961</v>
       </c>
       <c r="B62" s="1">
-        <v>55.658999999999999</v>
+        <v>55659</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>54</v>
@@ -1276,7 +1276,7 @@
         <v>1960</v>
       </c>
       <c r="B63" s="1">
-        <v>55.716999999999999</v>
+        <v>55717</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
Tasa de mortalidad, actualizacion 500
</commit_message>
<xml_diff>
--- a/Tasa de mortalidad.xlsx
+++ b/Tasa de mortalidad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moises Almanzar\Desktop\Proyecto Samsung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{224D975D-1F7A-4076-BA85-854DBF86CE98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A235AA-2DFE-44A0-956A-AFA129A719B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{40AD7953-8F09-4713-9AB9-62C2B40834AF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Fecha</t>
   </si>
@@ -45,165 +45,6 @@
   </si>
   <si>
     <t>Tasa mortalidad</t>
-  </si>
-  <si>
-    <t>6.68‰</t>
-  </si>
-  <si>
-    <t>6.46‰</t>
-  </si>
-  <si>
-    <t>6.01‰</t>
-  </si>
-  <si>
-    <t>6.06‰</t>
-  </si>
-  <si>
-    <t>6.03‰</t>
-  </si>
-  <si>
-    <t>5.96‰</t>
-  </si>
-  <si>
-    <t>5.88‰</t>
-  </si>
-  <si>
-    <t>5.83‰</t>
-  </si>
-  <si>
-    <t>5.80‰</t>
-  </si>
-  <si>
-    <t>5.84‰</t>
-  </si>
-  <si>
-    <t>5.82‰</t>
-  </si>
-  <si>
-    <t>5.86‰</t>
-  </si>
-  <si>
-    <t>5.87‰</t>
-  </si>
-  <si>
-    <t>5.93‰</t>
-  </si>
-  <si>
-    <t>6.09‰</t>
-  </si>
-  <si>
-    <t>6.20‰</t>
-  </si>
-  <si>
-    <t>6.17‰</t>
-  </si>
-  <si>
-    <t>5.78‰</t>
-  </si>
-  <si>
-    <t>5.70‰</t>
-  </si>
-  <si>
-    <t>5.62‰</t>
-  </si>
-  <si>
-    <t>5.69‰</t>
-  </si>
-  <si>
-    <t>5.79‰</t>
-  </si>
-  <si>
-    <t>5.92‰</t>
-  </si>
-  <si>
-    <t>6.08‰</t>
-  </si>
-  <si>
-    <t>6.26‰</t>
-  </si>
-  <si>
-    <t>6.45‰</t>
-  </si>
-  <si>
-    <t>6.94‰</t>
-  </si>
-  <si>
-    <t>7.23‰</t>
-  </si>
-  <si>
-    <t>7.52‰</t>
-  </si>
-  <si>
-    <t>7.81‰</t>
-  </si>
-  <si>
-    <t>8.08‰</t>
-  </si>
-  <si>
-    <t>8.39‰</t>
-  </si>
-  <si>
-    <t>8.71‰</t>
-  </si>
-  <si>
-    <t>9.17‰</t>
-  </si>
-  <si>
-    <t>9.12‰</t>
-  </si>
-  <si>
-    <t>9.36‰</t>
-  </si>
-  <si>
-    <t>9.62‰</t>
-  </si>
-  <si>
-    <t>9.90‰</t>
-  </si>
-  <si>
-    <t>10.21‰</t>
-  </si>
-  <si>
-    <t>10.52‰</t>
-  </si>
-  <si>
-    <t>10.81‰</t>
-  </si>
-  <si>
-    <t>11.11‰</t>
-  </si>
-  <si>
-    <t>11.49‰</t>
-  </si>
-  <si>
-    <t>11.99‰</t>
-  </si>
-  <si>
-    <t>12.51‰</t>
-  </si>
-  <si>
-    <t>13.07‰</t>
-  </si>
-  <si>
-    <t>13.62‰</t>
-  </si>
-  <si>
-    <t>15.14‰</t>
-  </si>
-  <si>
-    <t>14.66‰</t>
-  </si>
-  <si>
-    <t>15.32‰</t>
-  </si>
-  <si>
-    <t>15.77‰</t>
-  </si>
-  <si>
-    <t>16.33‰</t>
-  </si>
-  <si>
-    <t>16.89‰</t>
   </si>
 </sst>
 </file>
@@ -239,9 +80,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -581,7 +425,7 @@
   <dimension ref="A1:C63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B63"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -607,8 +451,8 @@
       <c r="B2" s="1">
         <v>74245</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
+      <c r="C2" s="2">
+        <v>6.6799999999999998E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -618,8 +462,8 @@
       <c r="B3" s="1">
         <v>71058</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
+      <c r="C3" s="2">
+        <v>6.4600000000000005E-2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
@@ -629,8 +473,8 @@
       <c r="B4" s="1">
         <v>6221</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
+      <c r="C4" s="2">
+        <v>6.0100000000000001E-2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
@@ -640,8 +484,8 @@
       <c r="B5" s="1">
         <v>62212</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>6</v>
+      <c r="C5" s="2">
+        <v>6.0600000000000001E-2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
@@ -651,8 +495,8 @@
       <c r="B6" s="1">
         <v>61339</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>7</v>
+      <c r="C6" s="2">
+        <v>6.0299999999999999E-2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
@@ -662,8 +506,8 @@
       <c r="B7" s="1">
         <v>60087</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>8</v>
+      <c r="C7" s="2">
+        <v>5.96E-2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
@@ -673,8 +517,8 @@
       <c r="B8" s="1">
         <v>58712</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>9</v>
+      <c r="C8" s="2">
+        <v>5.8799999999999998E-2</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
@@ -684,8 +528,8 @@
       <c r="B9" s="1">
         <v>57588</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>10</v>
+      <c r="C9" s="2">
+        <v>5.8299999999999998E-2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
@@ -695,8 +539,8 @@
       <c r="B10" s="1">
         <v>56782</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>11</v>
+      <c r="C10" s="2">
+        <v>5.8000000000000003E-2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
@@ -706,8 +550,8 @@
       <c r="B11" s="1">
         <v>56169</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>11</v>
+      <c r="C11" s="2">
+        <v>5.8000000000000003E-2</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
@@ -717,8 +561,8 @@
       <c r="B12" s="1">
         <v>55947</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>12</v>
+      <c r="C12" s="2">
+        <v>5.8400000000000001E-2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
@@ -728,8 +572,8 @@
       <c r="B13" s="1">
         <v>55177</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>13</v>
+      <c r="C13" s="2">
+        <v>5.8200000000000002E-2</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
@@ -739,8 +583,8 @@
       <c r="B14" s="1">
         <v>54695</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>10</v>
+      <c r="C14" s="2">
+        <v>5.8299999999999998E-2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
@@ -750,8 +594,8 @@
       <c r="B15" s="1">
         <v>54112</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>10</v>
+      <c r="C15" s="2">
+        <v>5.8299999999999998E-2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
@@ -761,8 +605,8 @@
       <c r="B16" s="1">
         <v>5375</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>14</v>
+      <c r="C16" s="2">
+        <v>5.8599999999999999E-2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
@@ -772,8 +616,8 @@
       <c r="B17" s="1">
         <v>53274</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>15</v>
+      <c r="C17" s="2">
+        <v>5.8700000000000002E-2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
@@ -783,8 +627,8 @@
       <c r="B18" s="1">
         <v>53207</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>16</v>
+      <c r="C18" s="2">
+        <v>5.9299999999999999E-2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
@@ -794,8 +638,8 @@
       <c r="B19" s="1">
         <v>53936</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>17</v>
+      <c r="C19" s="2">
+        <v>6.0900000000000003E-2</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
@@ -805,8 +649,8 @@
       <c r="B20" s="1">
         <v>53266</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>17</v>
+      <c r="C20" s="2">
+        <v>6.0900000000000003E-2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
@@ -816,8 +660,8 @@
       <c r="B21" s="1">
         <v>53511</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>18</v>
+      <c r="C21" s="2">
+        <v>6.2E-2</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
@@ -827,8 +671,8 @@
       <c r="B22" s="1">
         <v>52789</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>18</v>
+      <c r="C22" s="2">
+        <v>6.2E-2</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
@@ -838,8 +682,8 @@
       <c r="B23" s="1">
         <v>51807</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>19</v>
+      <c r="C23" s="2">
+        <v>6.1699999999999998E-2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
@@ -849,8 +693,8 @@
       <c r="B24" s="1">
         <v>50417</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>17</v>
+      <c r="C24" s="2">
+        <v>6.0900000000000003E-2</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
@@ -860,8 +704,8 @@
       <c r="B25" s="1">
         <v>49116</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>7</v>
+      <c r="C25" s="2">
+        <v>6.0299999999999999E-2</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
@@ -871,8 +715,8 @@
       <c r="B26" s="1">
         <v>47159</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>9</v>
+      <c r="C26" s="2">
+        <v>5.8799999999999998E-2</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
@@ -882,8 +726,8 @@
       <c r="B27" s="1">
         <v>45676</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>20</v>
+      <c r="C27" s="2">
+        <v>5.7799999999999997E-2</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
@@ -893,8 +737,8 @@
       <c r="B28" s="1">
         <v>44256</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>21</v>
+      <c r="C28" s="2">
+        <v>5.7000000000000002E-2</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.45">
@@ -904,8 +748,8 @@
       <c r="B29" s="1">
         <v>42979</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>22</v>
+      <c r="C29" s="2">
+        <v>5.62E-2</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.45">
@@ -915,8 +759,8 @@
       <c r="B30" s="1">
         <v>42768</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>23</v>
+      <c r="C30" s="2">
+        <v>5.6899999999999999E-2</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.45">
@@ -926,8 +770,8 @@
       <c r="B31" s="1">
         <v>42701</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>24</v>
+      <c r="C31" s="2">
+        <v>5.79E-2</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.45">
@@ -937,8 +781,8 @@
       <c r="B32" s="1">
         <v>42873</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>25</v>
+      <c r="C32" s="2">
+        <v>5.9200000000000003E-2</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.45">
@@ -948,8 +792,8 @@
       <c r="B33" s="1">
         <v>43263</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>26</v>
+      <c r="C33" s="2">
+        <v>6.08E-2</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.45">
@@ -959,8 +803,8 @@
       <c r="B34" s="1">
         <v>43675</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>27</v>
+      <c r="C34" s="2">
+        <v>6.2600000000000003E-2</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.45">
@@ -970,8 +814,8 @@
       <c r="B35" s="1">
         <v>44054</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>28</v>
+      <c r="C35" s="2">
+        <v>6.4500000000000002E-2</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.45">
@@ -981,8 +825,8 @@
       <c r="B36" s="1">
         <v>44536</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>3</v>
+      <c r="C36" s="2">
+        <v>6.6799999999999998E-2</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.45">
@@ -992,8 +836,8 @@
       <c r="B37" s="1">
         <v>45179</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>29</v>
+      <c r="C37" s="2">
+        <v>6.9400000000000003E-2</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.45">
@@ -1003,8 +847,8 @@
       <c r="B38" s="1">
         <v>45913</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>30</v>
+      <c r="C38" s="2">
+        <v>7.2300000000000003E-2</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.45">
@@ -1014,8 +858,8 @@
       <c r="B39" s="1">
         <v>46664</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>31</v>
+      <c r="C39" s="2">
+        <v>7.5200000000000003E-2</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.45">
@@ -1025,8 +869,8 @@
       <c r="B40" s="1">
         <v>47285</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>32</v>
+      <c r="C40" s="2">
+        <v>7.8100000000000003E-2</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.45">
@@ -1036,8 +880,8 @@
       <c r="B41" s="1">
         <v>47825</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>33</v>
+      <c r="C41" s="2">
+        <v>8.0799999999999997E-2</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.45">
@@ -1047,8 +891,8 @@
       <c r="B42" s="1">
         <v>48497</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>34</v>
+      <c r="C42" s="2">
+        <v>8.3900000000000002E-2</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.45">
@@ -1058,8 +902,8 @@
       <c r="B43" s="1">
         <v>4924</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>35</v>
+      <c r="C43" s="2">
+        <v>8.7099999999999997E-2</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.45">
@@ -1069,8 +913,8 @@
       <c r="B44" s="1">
         <v>51572</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>36</v>
+      <c r="C44" s="2">
+        <v>9.1700000000000004E-2</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.45">
@@ -1080,8 +924,8 @@
       <c r="B45" s="1">
         <v>50102</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>37</v>
+      <c r="C45" s="2">
+        <v>9.1200000000000003E-2</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.45">
@@ -1091,8 +935,8 @@
       <c r="B46" s="1">
         <v>50196</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>38</v>
+      <c r="C46" s="2">
+        <v>9.3600000000000003E-2</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.45">
@@ -1102,8 +946,8 @@
       <c r="B47" s="1">
         <v>50343</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>39</v>
+      <c r="C47" s="2">
+        <v>9.6199999999999994E-2</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.45">
@@ -1113,8 +957,8 @@
       <c r="B48" s="1">
         <v>50544</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>40</v>
+      <c r="C48" s="2">
+        <v>9.9000000000000005E-2</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.45">
@@ -1124,8 +968,8 @@
       <c r="B49" s="1">
         <v>50821</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>41</v>
+      <c r="C49" s="2">
+        <v>0.1021</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.45">
@@ -1135,8 +979,8 @@
       <c r="B50" s="1">
         <v>51025</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>42</v>
+      <c r="C50" s="2">
+        <v>0.1052</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.45">
@@ -1146,8 +990,8 @@
       <c r="B51" s="1">
         <v>51066</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>43</v>
+      <c r="C51" s="2">
+        <v>0.1081</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.45">
@@ -1157,8 +1001,8 @@
       <c r="B52" s="1">
         <v>51081</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>44</v>
+      <c r="C52" s="2">
+        <v>0.1111</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.45">
@@ -1168,8 +1012,8 @@
       <c r="B53" s="1">
         <v>51437</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>45</v>
+      <c r="C53" s="2">
+        <v>0.1149</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.45">
@@ -1179,8 +1023,8 @@
       <c r="B54" s="1">
         <v>5217</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>46</v>
+      <c r="C54" s="2">
+        <v>0.11990000000000001</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.45">
@@ -1190,8 +1034,8 @@
       <c r="B55" s="1">
         <v>52941</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>47</v>
+      <c r="C55" s="2">
+        <v>0.12509999999999999</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.45">
@@ -1201,8 +1045,8 @@
       <c r="B56" s="1">
         <v>53687</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>48</v>
+      <c r="C56" s="2">
+        <v>0.13070000000000001</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.45">
@@ -1212,8 +1056,8 @@
       <c r="B57" s="1">
         <v>543</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>49</v>
+      <c r="C57" s="2">
+        <v>0.13619999999999999</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.45">
@@ -1223,8 +1067,8 @@
       <c r="B58" s="1">
         <v>58565</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>50</v>
+      <c r="C58" s="2">
+        <v>0.15140000000000001</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.45">
@@ -1234,8 +1078,8 @@
       <c r="B59" s="1">
         <v>54998</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>51</v>
+      <c r="C59" s="2">
+        <v>0.14660000000000001</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.45">
@@ -1245,8 +1089,8 @@
       <c r="B60" s="1">
         <v>55704</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>52</v>
+      <c r="C60" s="2">
+        <v>0.1532</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.45">
@@ -1256,8 +1100,8 @@
       <c r="B61" s="1">
         <v>55515</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>53</v>
+      <c r="C61" s="2">
+        <v>0.15770000000000001</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.45">
@@ -1267,8 +1111,8 @@
       <c r="B62" s="1">
         <v>55659</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>54</v>
+      <c r="C62" s="2">
+        <v>0.1633</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.45">
@@ -1278,8 +1122,8 @@
       <c r="B63" s="1">
         <v>55717</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>55</v>
+      <c r="C63" s="2">
+        <v>0.16889999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tasa de mortalidad, update de nuevo
</commit_message>
<xml_diff>
--- a/Tasa de mortalidad.xlsx
+++ b/Tasa de mortalidad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moises Almanzar\Desktop\Proyecto Samsung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A235AA-2DFE-44A0-956A-AFA129A719B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B378AAB8-5175-4822-8DBE-C4E89BA4B4C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{40AD7953-8F09-4713-9AB9-62C2B40834AF}"/>
   </bookViews>
@@ -425,7 +425,7 @@
   <dimension ref="A1:C63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -471,7 +471,7 @@
         <v>2019</v>
       </c>
       <c r="B4" s="1">
-        <v>6221</v>
+        <v>62210</v>
       </c>
       <c r="C4" s="2">
         <v>6.0100000000000001E-2</v>
@@ -603,7 +603,7 @@
         <v>2007</v>
       </c>
       <c r="B16" s="1">
-        <v>5375</v>
+        <v>53750</v>
       </c>
       <c r="C16" s="2">
         <v>5.8599999999999999E-2</v>
@@ -900,7 +900,7 @@
         <v>1980</v>
       </c>
       <c r="B43" s="1">
-        <v>4924</v>
+        <v>49240</v>
       </c>
       <c r="C43" s="2">
         <v>8.7099999999999997E-2</v>
@@ -1021,7 +1021,7 @@
         <v>1969</v>
       </c>
       <c r="B54" s="1">
-        <v>5217</v>
+        <v>52170</v>
       </c>
       <c r="C54" s="2">
         <v>0.11990000000000001</v>
@@ -1054,7 +1054,7 @@
         <v>1966</v>
       </c>
       <c r="B57" s="1">
-        <v>543</v>
+        <v>54300</v>
       </c>
       <c r="C57" s="2">
         <v>0.13619999999999999</v>

</xml_diff>